<commit_message>
finished generator dokumen refactors
</commit_message>
<xml_diff>
--- a/dokumen_pendukung/templates/templateInvoiceFinal.xlsx
+++ b/dokumen_pendukung/templates/templateInvoiceFinal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\honeyn\Documents\PROPEN\SIAP-BE\siap-be\dokumen_pendukung\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HANIN\Documents\SIAP_LSI\siap-be\dokumen_pendukung\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CC3F3F-97FE-4690-AE1E-B151A8FD4419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B0DC1F-6819-40AE-9FCB-30686D57CAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dapil Gerindra LSI" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Inv No: ___/SURV/LSI/IX/2024</t>
   </si>
@@ -139,21 +139,36 @@
   <si>
     <t xml:space="preserve">INVOICE PEMBAYARAN PELUNASAN SURVEI : </t>
   </si>
+  <si>
+    <t>Bank Swift Code</t>
+  </si>
+  <si>
+    <t>Tax ID</t>
+  </si>
+  <si>
+    <t>Best Regards,</t>
+  </si>
+  <si>
+    <t>Gadis Gustika Y</t>
+  </si>
+  <si>
+    <t>Finance Dept</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;Rp&quot;* #,##0_);_(&quot;Rp&quot;* \(#,##0\);_(&quot;Rp&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="[$Rp-421]#,##0;\-[$Rp-421]#,##0"/>
-    <numFmt numFmtId="169" formatCode="&quot;Rp&quot;#,##0_);[Red]\(&quot;Rp&quot;#,##0\)"/>
-    <numFmt numFmtId="170" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;Rp&quot;* #,##0_);_(&quot;Rp&quot;* \(#,##0\);_(&quot;Rp&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$Rp-421]#,##0;\-[$Rp-421]#,##0"/>
+    <numFmt numFmtId="168" formatCode="&quot;Rp&quot;#,##0_);[Red]\(&quot;Rp&quot;#,##0\)"/>
+    <numFmt numFmtId="169" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +246,20 @@
       <sz val="12"/>
       <color rgb="FF486166"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -598,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -632,7 +661,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -642,8 +671,8 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -669,10 +698,10 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -681,7 +710,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -690,13 +719,13 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -711,17 +740,17 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -744,10 +773,32 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -760,29 +811,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,40 +889,6 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="400050" cy="219075"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="image2.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1107,37 +1105,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.86328125" customWidth="1"/>
-    <col min="2" max="2" width="15.265625" customWidth="1"/>
-    <col min="3" max="3" width="4.265625" customWidth="1"/>
-    <col min="4" max="4" width="14.265625" customWidth="1"/>
-    <col min="5" max="5" width="26.265625" customWidth="1"/>
-    <col min="6" max="6" width="6.53125" customWidth="1"/>
-    <col min="7" max="7" width="20.265625" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="26.21875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="0.3984375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0.44140625" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="15" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1328125" customWidth="1"/>
-    <col min="13" max="26" width="9.1328125" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" customWidth="1"/>
+    <col min="13" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A1" s="93"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1157,15 +1155,15 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1185,15 +1183,15 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A3" s="74"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
+      <c r="A3" s="78"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1213,15 +1211,15 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A4" s="74"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
+      <c r="A4" s="78"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1241,15 +1239,15 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1269,15 +1267,15 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A6" s="74"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1297,15 +1295,15 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A7" s="74"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
+      <c r="A7" s="78"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="78"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1331,8 +1329,8 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="74"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="78"/>
       <c r="I8" s="5"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1361,8 +1359,8 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1389,8 +1387,8 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1417,8 +1415,8 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1445,8 +1443,8 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1499,14 +1497,14 @@
       <c r="B14" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="88"/>
-      <c r="D14" s="89"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="74"/>
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="91" t="s">
+      <c r="G14" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="74"/>
+      <c r="H14" s="78"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1561,10 +1559,10 @@
       <c r="B16" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="90"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="89"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="74"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="1"/>
@@ -1760,12 +1758,12 @@
       <c r="A23" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="84"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="82"/>
       <c r="F23" s="30" t="s">
         <v>8</v>
       </c>
@@ -1854,12 +1852,12 @@
       <c r="A26" s="40">
         <v>1</v>
       </c>
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="87"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="85"/>
       <c r="F26" s="41"/>
       <c r="G26" s="42"/>
       <c r="H26" s="43"/>
@@ -1884,12 +1882,12 @@
     </row>
     <row r="27" spans="1:26" ht="15" customHeight="1">
       <c r="A27" s="44"/>
-      <c r="B27" s="73" t="s">
+      <c r="B27" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="75"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="87"/>
       <c r="F27" s="45">
         <v>0.6</v>
       </c>
@@ -1919,10 +1917,10 @@
     </row>
     <row r="28" spans="1:26" ht="15" customHeight="1">
       <c r="A28" s="44"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="75"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="87"/>
       <c r="F28" s="45"/>
       <c r="G28" s="43"/>
       <c r="H28" s="46"/>
@@ -1947,10 +1945,10 @@
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
       <c r="A29" s="47"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="75"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="87"/>
       <c r="F29" s="48"/>
       <c r="G29" s="49"/>
       <c r="H29" s="43"/>
@@ -1975,10 +1973,10 @@
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
       <c r="A30" s="47"/>
-      <c r="B30" s="73"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="75"/>
+      <c r="B30" s="86"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="87"/>
       <c r="F30" s="48"/>
       <c r="G30" s="50"/>
       <c r="H30" s="51"/>
@@ -2003,12 +2001,12 @@
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1">
       <c r="A31" s="47"/>
-      <c r="B31" s="73" t="s">
+      <c r="B31" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="75"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="87"/>
       <c r="F31" s="48"/>
       <c r="G31" s="50"/>
       <c r="H31" s="51"/>
@@ -2061,14 +2059,14 @@
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
       <c r="A33" s="58"/>
-      <c r="B33" s="76" t="s">
+      <c r="B33" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="78"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="90"/>
       <c r="H33" s="59">
         <f>SUM(H26:H32)</f>
         <v>0</v>
@@ -2125,14 +2123,14 @@
       <c r="B35" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="79" t="s">
+      <c r="C35" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="74"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2155,11 +2153,11 @@
     <row r="36" spans="1:26" ht="18.75" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="61"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
+      <c r="C36" s="92"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
       <c r="H36" s="62"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2187,9 +2185,11 @@
       <c r="D37" s="1"/>
       <c r="E37" s="63"/>
       <c r="F37" s="11"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
+      <c r="G37" s="93"/>
+      <c r="H37" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="94"/>
       <c r="J37" s="28"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -2217,9 +2217,9 @@
       <c r="D38" s="65"/>
       <c r="E38" s="66"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="95"/>
+      <c r="I38" s="94"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -2249,9 +2249,9 @@
       <c r="D39" s="67"/>
       <c r="E39" s="66"/>
       <c r="F39" s="11"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="74"/>
+      <c r="G39" s="94"/>
+      <c r="H39" s="95"/>
+      <c r="I39" s="94"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -2281,9 +2281,9 @@
       <c r="D40" s="67"/>
       <c r="E40" s="66"/>
       <c r="F40" s="11"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="74"/>
+      <c r="G40" s="94"/>
+      <c r="H40" s="95"/>
+      <c r="I40" s="94"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -2313,9 +2313,9 @@
       <c r="D41" s="67"/>
       <c r="E41" s="66"/>
       <c r="F41" s="11"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
+      <c r="G41" s="94"/>
+      <c r="H41" s="95"/>
+      <c r="I41" s="94"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -2345,9 +2345,9 @@
       <c r="D42" s="67"/>
       <c r="E42" s="66"/>
       <c r="F42" s="11"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
+      <c r="G42" s="94"/>
+      <c r="H42" s="95"/>
+      <c r="I42" s="94"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -2377,9 +2377,11 @@
       <c r="D43" s="67"/>
       <c r="E43" s="66"/>
       <c r="F43" s="11"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="74"/>
+      <c r="G43" s="94"/>
+      <c r="H43" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="I43" s="94"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -2400,14 +2402,18 @@
     </row>
     <row r="44" spans="1:26" ht="12.75" customHeight="1">
       <c r="A44" s="1"/>
-      <c r="B44" s="70"/>
+      <c r="B44" s="70" t="s">
+        <v>28</v>
+      </c>
       <c r="C44" s="7"/>
       <c r="D44" s="1"/>
       <c r="E44" s="63"/>
       <c r="F44" s="11"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="74"/>
-      <c r="I44" s="74"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="I44" s="94"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -2428,14 +2434,16 @@
     </row>
     <row r="45" spans="1:26" ht="12.75" customHeight="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C45" s="70"/>
       <c r="D45" s="1"/>
       <c r="E45" s="63"/>
       <c r="F45" s="11"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
+      <c r="G45" s="94"/>
+      <c r="H45" s="94"/>
+      <c r="I45" s="94"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -29193,13 +29201,7 @@
       <c r="Z1000" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G8:H12"/>
-    <mergeCell ref="A1:I7"/>
-    <mergeCell ref="G37:I45"/>
+  <mergeCells count="15">
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B27:E27"/>
@@ -29210,6 +29212,11 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="C35:H35"/>
     <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G8:H12"/>
+    <mergeCell ref="A1:I7"/>
   </mergeCells>
   <pageMargins left="0.70902777777777803" right="0.15902777777777799" top="0.78888888888888897" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'dev' into pengendali-mutu"
This reverts commit 378197f84c8119be4cd35af23656d6c98ee8a48c, reversing
changes made to cf71de0760332db8ec8535ae5fd68448eee09165.
</commit_message>
<xml_diff>
--- a/dokumen_pendukung/templates/templateInvoiceFinal.xlsx
+++ b/dokumen_pendukung/templates/templateInvoiceFinal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HANIN\Documents\SIAP_LSI\siap-be\dokumen_pendukung\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\honeyn\Documents\PROPEN\SIAP-BE\siap-be\dokumen_pendukung\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B0DC1F-6819-40AE-9FCB-30686D57CAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CC3F3F-97FE-4690-AE1E-B151A8FD4419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dapil Gerindra LSI" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Inv No: ___/SURV/LSI/IX/2024</t>
   </si>
@@ -139,36 +139,21 @@
   <si>
     <t xml:space="preserve">INVOICE PEMBAYARAN PELUNASAN SURVEI : </t>
   </si>
-  <si>
-    <t>Bank Swift Code</t>
-  </si>
-  <si>
-    <t>Tax ID</t>
-  </si>
-  <si>
-    <t>Best Regards,</t>
-  </si>
-  <si>
-    <t>Gadis Gustika Y</t>
-  </si>
-  <si>
-    <t>Finance Dept</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;Rp&quot;* #,##0_);_(&quot;Rp&quot;* \(#,##0\);_(&quot;Rp&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$Rp-421]#,##0;\-[$Rp-421]#,##0"/>
-    <numFmt numFmtId="168" formatCode="&quot;Rp&quot;#,##0_);[Red]\(&quot;Rp&quot;#,##0\)"/>
-    <numFmt numFmtId="169" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;Rp&quot;* #,##0_);_(&quot;Rp&quot;* \(#,##0\);_(&quot;Rp&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="[$Rp-421]#,##0;\-[$Rp-421]#,##0"/>
+    <numFmt numFmtId="169" formatCode="&quot;Rp&quot;#,##0_);[Red]\(&quot;Rp&quot;#,##0\)"/>
+    <numFmt numFmtId="170" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,20 +231,6 @@
       <sz val="12"/>
       <color rgb="FF486166"/>
       <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -627,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -661,7 +632,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -671,8 +642,8 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -698,10 +669,10 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -710,7 +681,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -719,13 +690,13 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -740,17 +711,17 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -773,32 +744,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -811,10 +760,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,6 +857,40 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="219075"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="image2.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1105,37 +1107,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="4.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="26.21875" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.86328125" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" customWidth="1"/>
+    <col min="3" max="3" width="4.265625" customWidth="1"/>
+    <col min="4" max="4" width="14.265625" customWidth="1"/>
+    <col min="5" max="5" width="26.265625" customWidth="1"/>
+    <col min="6" max="6" width="6.53125" customWidth="1"/>
+    <col min="7" max="7" width="20.265625" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="0.44140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0.3984375" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="15" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" customWidth="1"/>
-    <col min="13" max="26" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="14.1328125" customWidth="1"/>
+    <col min="13" max="26" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A1" s="80"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
+      <c r="A1" s="93"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1155,15 +1157,15 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1183,15 +1185,15 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A3" s="78"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1211,15 +1213,15 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A4" s="78"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1239,15 +1241,15 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A5" s="78"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1267,15 +1269,15 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A6" s="78"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1295,15 +1297,15 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A7" s="78"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
+      <c r="A7" s="74"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1329,8 +1331,8 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="78"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="74"/>
       <c r="I8" s="5"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1359,8 +1361,8 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1387,8 +1389,8 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="78"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1415,8 +1417,8 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1443,8 +1445,8 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1497,14 +1499,14 @@
       <c r="B14" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="74"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="89"/>
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="77" t="s">
+      <c r="G14" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="78"/>
+      <c r="H14" s="74"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1559,10 +1561,10 @@
       <c r="B16" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="74"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="89"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="1"/>
@@ -1758,12 +1760,12 @@
       <c r="A23" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="82"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="84"/>
       <c r="F23" s="30" t="s">
         <v>8</v>
       </c>
@@ -1852,12 +1854,12 @@
       <c r="A26" s="40">
         <v>1</v>
       </c>
-      <c r="B26" s="83" t="s">
+      <c r="B26" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="85"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="87"/>
       <c r="F26" s="41"/>
       <c r="G26" s="42"/>
       <c r="H26" s="43"/>
@@ -1882,12 +1884,12 @@
     </row>
     <row r="27" spans="1:26" ht="15" customHeight="1">
       <c r="A27" s="44"/>
-      <c r="B27" s="86" t="s">
+      <c r="B27" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="87"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="75"/>
       <c r="F27" s="45">
         <v>0.6</v>
       </c>
@@ -1917,10 +1919,10 @@
     </row>
     <row r="28" spans="1:26" ht="15" customHeight="1">
       <c r="A28" s="44"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="87"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="75"/>
       <c r="F28" s="45"/>
       <c r="G28" s="43"/>
       <c r="H28" s="46"/>
@@ -1945,10 +1947,10 @@
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
       <c r="A29" s="47"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="87"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="75"/>
       <c r="F29" s="48"/>
       <c r="G29" s="49"/>
       <c r="H29" s="43"/>
@@ -1973,10 +1975,10 @@
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
       <c r="A30" s="47"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="87"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="75"/>
       <c r="F30" s="48"/>
       <c r="G30" s="50"/>
       <c r="H30" s="51"/>
@@ -2001,12 +2003,12 @@
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1">
       <c r="A31" s="47"/>
-      <c r="B31" s="86" t="s">
+      <c r="B31" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="87"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="75"/>
       <c r="F31" s="48"/>
       <c r="G31" s="50"/>
       <c r="H31" s="51"/>
@@ -2059,14 +2061,14 @@
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
       <c r="A33" s="58"/>
-      <c r="B33" s="88" t="s">
+      <c r="B33" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="89"/>
-      <c r="D33" s="89"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="89"/>
-      <c r="G33" s="90"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="78"/>
       <c r="H33" s="59">
         <f>SUM(H26:H32)</f>
         <v>0</v>
@@ -2123,14 +2125,14 @@
       <c r="B35" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="91" t="s">
+      <c r="C35" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2153,11 +2155,11 @@
     <row r="36" spans="1:26" ht="18.75" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="61"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
       <c r="H36" s="62"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2185,11 +2187,9 @@
       <c r="D37" s="1"/>
       <c r="E37" s="63"/>
       <c r="F37" s="11"/>
-      <c r="G37" s="93"/>
-      <c r="H37" s="95" t="s">
-        <v>30</v>
-      </c>
-      <c r="I37" s="94"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="74"/>
       <c r="J37" s="28"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -2217,9 +2217,9 @@
       <c r="D38" s="65"/>
       <c r="E38" s="66"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="94"/>
-      <c r="H38" s="95"/>
-      <c r="I38" s="94"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -2249,9 +2249,9 @@
       <c r="D39" s="67"/>
       <c r="E39" s="66"/>
       <c r="F39" s="11"/>
-      <c r="G39" s="94"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="94"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -2281,9 +2281,9 @@
       <c r="D40" s="67"/>
       <c r="E40" s="66"/>
       <c r="F40" s="11"/>
-      <c r="G40" s="94"/>
-      <c r="H40" s="95"/>
-      <c r="I40" s="94"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="74"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -2313,9 +2313,9 @@
       <c r="D41" s="67"/>
       <c r="E41" s="66"/>
       <c r="F41" s="11"/>
-      <c r="G41" s="94"/>
-      <c r="H41" s="95"/>
-      <c r="I41" s="94"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -2345,9 +2345,9 @@
       <c r="D42" s="67"/>
       <c r="E42" s="66"/>
       <c r="F42" s="11"/>
-      <c r="G42" s="94"/>
-      <c r="H42" s="95"/>
-      <c r="I42" s="94"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -2377,11 +2377,9 @@
       <c r="D43" s="67"/>
       <c r="E43" s="66"/>
       <c r="F43" s="11"/>
-      <c r="G43" s="94"/>
-      <c r="H43" s="96" t="s">
-        <v>31</v>
-      </c>
-      <c r="I43" s="94"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -2402,18 +2400,14 @@
     </row>
     <row r="44" spans="1:26" ht="12.75" customHeight="1">
       <c r="A44" s="1"/>
-      <c r="B44" s="70" t="s">
-        <v>28</v>
-      </c>
+      <c r="B44" s="70"/>
       <c r="C44" s="7"/>
       <c r="D44" s="1"/>
       <c r="E44" s="63"/>
       <c r="F44" s="11"/>
-      <c r="G44" s="94"/>
-      <c r="H44" s="95" t="s">
-        <v>32</v>
-      </c>
-      <c r="I44" s="94"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="74"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -2434,16 +2428,14 @@
     </row>
     <row r="45" spans="1:26" ht="12.75" customHeight="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B45" s="1"/>
       <c r="C45" s="70"/>
       <c r="D45" s="1"/>
       <c r="E45" s="63"/>
       <c r="F45" s="11"/>
-      <c r="G45" s="94"/>
-      <c r="H45" s="94"/>
-      <c r="I45" s="94"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="74"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -29201,7 +29193,13 @@
       <c r="Z1000" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G8:H12"/>
+    <mergeCell ref="A1:I7"/>
+    <mergeCell ref="G37:I45"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B27:E27"/>
@@ -29212,11 +29210,6 @@
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="C35:H35"/>
     <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G8:H12"/>
-    <mergeCell ref="A1:I7"/>
   </mergeCells>
   <pageMargins left="0.70902777777777803" right="0.15902777777777799" top="0.78888888888888897" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait"/>

</xml_diff>